<commit_message>
validacion de casos nuevo e hijos
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\88891\Documents\UiPath\Archivaldo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15C5B39-B69A-4E47-8987-92A8590243DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B848C34B-6DF1-4479-BBC6-9A7853DCB3BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
integracion del analisis de documentos
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beecker\Documents\UiPath\ArchivaldoBot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\88891\Documents\UiPath\Archivaldo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E85BB0-67DA-4E84-B5E3-3C03B5735167}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="4740" yWindow="1740" windowWidth="16200" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -197,9 +198,6 @@
     <t>ContrasenaSalesforce</t>
   </si>
   <si>
-    <t>BdBancos.xlsx</t>
-  </si>
-  <si>
     <t>PathBDBancos</t>
   </si>
   <si>
@@ -219,12 +217,15 @@
   </si>
   <si>
     <t>C:\Users\Beecker\Documents\UiPath\Archivaldo\Data\ArchivosTmpCliente\</t>
+  </si>
+  <si>
+    <t>Data\Bancos_Aceptados.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -606,11 +607,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -721,37 +722,39 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
         <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1740,8 +1743,8 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1749,7 +1752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2962,7 +2965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Validacion de flujo general
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\88891\Documents\UiPath\Archivaldo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beecker\Documents\UiPath\ArchivaldoBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D21D8-5247-4082-A3FD-E3147B164EE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -219,13 +218,13 @@
     <t>Data\Bancos_Aceptados.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\88891\Documents\UiPath\Archivaldo\Data\ArchivosTmpCliente\</t>
+    <t>C:\Users\Beecker\Documents\UiPath\ArchivaldoBot\Data\ArchivosTmpCliente\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -607,11 +606,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1743,8 +1742,8 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1752,7 +1751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2965,7 +2964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Construccion de correo de respuesta construido
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -254,9 +254,6 @@
     <t>MensajeActividadLaboral</t>
   </si>
   <si>
-    <t>Asegurece de proporcionar los datos solicitado del beneficiario, esto a pesar de que usted sea el unico beneficiario</t>
-  </si>
-  <si>
     <t>MensajeVinculoPatrimonialRFC</t>
   </si>
   <si>
@@ -323,12 +320,6 @@
     <t>MensajeCartaAcreditacionDomicilioFiscal</t>
   </si>
   <si>
-    <t>Proporcione su comprobante de domicilio fiscal vigente</t>
-  </si>
-  <si>
-    <t>Envie su comprobante residencial vigente</t>
-  </si>
-  <si>
     <t>La direccion que viene en su comprobante de domicilio residencial no coincide con la registrada en GBM, por favor envie un comprobante donde coincidan su direccion residencial y nombre , o en su defecto envie su carta de acreditamiento de domicilio en formato pdf, misma que adjunto en este correo.</t>
   </si>
   <si>
@@ -341,12 +332,6 @@
     <t>El nombre en el comprobante de domicilio residencial que proporciono no esta a su nombre, por favor envie un comprobante donde coincidan su direccion residencial y nombre , o en su defecto envie su carta de acreditamiento de domicilio en formato pdf, misma que adjunto en este correo.</t>
   </si>
   <si>
-    <t>Llene completamente su carta de acreditacion de domicilio residencial</t>
-  </si>
-  <si>
-    <t>Llene completamente su carta de acreditacion de domicilio fiscal</t>
-  </si>
-  <si>
     <t>MensajeIdentificacion</t>
   </si>
   <si>
@@ -356,9 +341,6 @@
     <t>MensajeIdentificacionIlegible</t>
   </si>
   <si>
-    <t>La identificacion que proporciono es ilegible por favor escanee su identificacion y enviela de formato pdf</t>
-  </si>
-  <si>
     <t>MensajeCedulaInvalida</t>
   </si>
   <si>
@@ -368,9 +350,6 @@
     <t>MensajeINENoVigente</t>
   </si>
   <si>
-    <t>la identificacion que nos proporciono no esta vigente</t>
-  </si>
-  <si>
     <t>MensajeBancoEstadoCuenta</t>
   </si>
   <si>
@@ -380,21 +359,12 @@
     <t>MensajeNombreEstadoCuenta</t>
   </si>
   <si>
-    <t>El Estado de cuenta que proporciono no le pertence, por favor proporcione un estado de cuenta a su nombre por favor</t>
-  </si>
-  <si>
     <t>MensajeCuentaClabeEstadoCuenta</t>
   </si>
   <si>
-    <t>La cuenta clabe en el estado de cuenta que proporciono no coincide con la cuenta clabe que proporciono en GBM, por favor verifique</t>
-  </si>
-  <si>
     <t>MensajeEstadoCuenta</t>
   </si>
   <si>
-    <t>Por favor envie su estado de cuenta vigente</t>
-  </si>
-  <si>
     <t>PathAcreditacionDocumento</t>
   </si>
   <si>
@@ -405,6 +375,48 @@
   </si>
   <si>
     <t>C:\Users\Beecker\Documents\UiPath\ArchivaldoBot\Data\ArchivosEnviados\</t>
+  </si>
+  <si>
+    <t>Asegurece de llenar todos los campos de la seccion de Beneficiario, esto a pesar de que usted sea el beneficiario.</t>
+  </si>
+  <si>
+    <t>La identificacion que proporciono es ilegible por favor escanee su identificacion y enviela en formato pdf.</t>
+  </si>
+  <si>
+    <t>la identificacion que nos proporciono no esta vigente.</t>
+  </si>
+  <si>
+    <t>Por favor envie su estado de cuenta vigente.</t>
+  </si>
+  <si>
+    <t>La cuenta clabe en el estado de cuenta que proporciono no coincide con la cuenta clabe que proporciono en GBM, por favor verifique.</t>
+  </si>
+  <si>
+    <t>Llene completamente su carta de acreditacion de domicilio fiscal.</t>
+  </si>
+  <si>
+    <t>Llene completamente su carta de acreditacion de domicilio residencial.</t>
+  </si>
+  <si>
+    <t>Envie su comprobante residencial vigente.</t>
+  </si>
+  <si>
+    <t>Proporcione su comprobante de domicilio fiscal vigente.</t>
+  </si>
+  <si>
+    <t>MensajeProblemasSolicitud</t>
+  </si>
+  <si>
+    <t>El Estado de cuenta que proporciono no le pertence, por favor proporcione un estado de cuenta a su nombre por favor.</t>
+  </si>
+  <si>
+    <t>Tuvimos problemas validando su solicitud, por favor atienda las siguientes instrucciones:</t>
+  </si>
+  <si>
+    <t>MensajeProblemasDoctos</t>
+  </si>
+  <si>
+    <t>Tuvimos problemas validando los documentos que envio, a continuacion se enlistan:</t>
   </si>
 </sst>
 </file>
@@ -795,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -939,18 +951,18 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1952,8 +1964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2188,15 +2200,15 @@
         <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2204,7 +2216,7 @@
         <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2212,7 +2224,7 @@
         <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2220,7 +2232,7 @@
         <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2228,7 +2240,7 @@
         <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2236,7 +2248,7 @@
         <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2244,7 +2256,7 @@
         <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2252,7 +2264,7 @@
         <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2260,7 +2272,7 @@
         <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,7 +2280,7 @@
         <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2276,147 +2288,161 @@
         <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
         <v>90</v>
-      </c>
-      <c r="B39" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>